<commit_message>
Added support for no b-frames, removed post-encoding calculation of psnr
</commit_message>
<xml_diff>
--- a/python/tractor_stats.xlsx
+++ b/python/tractor_stats.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>target_bitrate_kbps</t>
   </si>
@@ -174,11 +175,65 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>other_kbps</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>49.403799999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.776799999999902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.6768</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.798499999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42.959899999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0487-4195-BD08-A949B80F8897}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$C$1</c:f>
@@ -200,30 +255,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>325</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>300</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$6</c:f>
@@ -234,7 +265,7 @@
                   <c:v>160.93860000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>154.36539999999999</c:v>
+                  <c:v>154.166</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>144.9213</c:v>
@@ -250,13 +281,13 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9A00-43BB-97B1-740D6565FAC0}"/>
+              <c16:uniqueId val="{00000000-0487-4195-BD08-A949B80F8897}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$D$1</c:f>
@@ -278,30 +309,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>325</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>300</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$6</c:f>
@@ -312,7 +319,7 @@
                   <c:v>178.416</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>162.94120000000001</c:v>
+                  <c:v>163.09800000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>149.51230000000001</c:v>
@@ -328,85 +335,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9A00-43BB-97B1-740D6565FAC0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>other_kbps</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>325</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>300</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$2:$E$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>49.406199999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>48.5062</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>46.679199999999902</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44.800899999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42.962299999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9A00-43BB-97B1-740D6565FAC0}"/>
+              <c16:uniqueId val="{00000001-0487-4195-BD08-A949B80F8897}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -419,7 +348,6 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
         <c:axId val="551460528"/>
         <c:axId val="551457904"/>
       </c:barChart>
@@ -607,7 +535,487 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Tractor Video, 10 Seconds, 1 I Frame, No B Frames, 25fps</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>other_kbps</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>62.270699999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.631399999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.760799999999897</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.869799999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.7179</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6D8F-4640-B183-86EC99C9678B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>prediction_kbps</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>167.7329</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>160.328</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>151.97880000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>146.1568</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>140.22559999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6D8F-4640-B183-86EC99C9678B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>residual_kbps</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>165.946</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150.84219999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>135.626</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>123.107</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>116.687699999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6D8F-4640-B183-86EC99C9678B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="560306112"/>
+        <c:axId val="560306440"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="560306112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="560306440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="560306440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="560306112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1152,19 +1560,559 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>36</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1189,6 +2137,22 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G6" totalsRowShown="0">
+  <autoFilter ref="A1:G6"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="target_bitrate_kbps"/>
+    <tableColumn id="2" name="achieved_bitrate_kbps"/>
+    <tableColumn id="3" name="prediction_kbps"/>
+    <tableColumn id="4" name="residual_kbps"/>
+    <tableColumn id="5" name="other_kbps"/>
+    <tableColumn id="6" name="avg_psnr"/>
+    <tableColumn id="7" name="avg_qp"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G6" totalsRowShown="0">
   <autoFilter ref="A1:G6"/>
   <tableColumns count="7">
     <tableColumn id="1" name="target_bitrate_kbps"/>
@@ -1468,8 +2432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,7 +2475,7 @@
         <v>400</v>
       </c>
       <c r="B2">
-        <v>388.76080000000002</v>
+        <v>388.75839999999999</v>
       </c>
       <c r="C2">
         <v>160.93860000000001</v>
@@ -1520,10 +2484,10 @@
         <v>178.416</v>
       </c>
       <c r="E2">
-        <v>49.406199999999998</v>
+        <v>49.403799999999997</v>
       </c>
       <c r="F2">
-        <v>33.049218000000003</v>
+        <v>33.311999999999998</v>
       </c>
       <c r="G2">
         <v>47.14</v>
@@ -1534,19 +2498,19 @@
         <v>375</v>
       </c>
       <c r="B3">
-        <v>365.81279999999998</v>
+        <v>366.04079999999999</v>
       </c>
       <c r="C3">
-        <v>154.36539999999999</v>
+        <v>154.166</v>
       </c>
       <c r="D3">
-        <v>162.94120000000001</v>
+        <v>163.09800000000001</v>
       </c>
       <c r="E3">
-        <v>48.5062</v>
+        <v>48.776799999999902</v>
       </c>
       <c r="F3">
-        <v>32.726643000000003</v>
+        <v>33.006</v>
       </c>
       <c r="G3">
         <v>47.6</v>
@@ -1557,7 +2521,7 @@
         <v>350</v>
       </c>
       <c r="B4">
-        <v>341.11279999999999</v>
+        <v>341.110399999999</v>
       </c>
       <c r="C4">
         <v>144.9213</v>
@@ -1566,10 +2530,10 @@
         <v>149.51230000000001</v>
       </c>
       <c r="E4">
-        <v>46.679199999999902</v>
+        <v>46.6768</v>
       </c>
       <c r="F4">
-        <v>32.358319000000002</v>
+        <v>32.631999999999998</v>
       </c>
       <c r="G4">
         <v>48.13</v>
@@ -1580,7 +2544,7 @@
         <v>325</v>
       </c>
       <c r="B5">
-        <v>318.72399999999999</v>
+        <v>318.721599999999</v>
       </c>
       <c r="C5">
         <v>137.14839999999899</v>
@@ -1589,10 +2553,10 @@
         <v>136.7747</v>
       </c>
       <c r="E5">
-        <v>44.800899999999999</v>
+        <v>44.798499999999997</v>
       </c>
       <c r="F5">
-        <v>32.049413999999999</v>
+        <v>32.32</v>
       </c>
       <c r="G5">
         <v>48.59</v>
@@ -1603,7 +2567,7 @@
         <v>300</v>
       </c>
       <c r="B6">
-        <v>298.26319999999998</v>
+        <v>298.26080000000002</v>
       </c>
       <c r="C6">
         <v>131.28440000000001</v>
@@ -1612,13 +2576,179 @@
         <v>124.01649999999999</v>
       </c>
       <c r="E6">
-        <v>42.962299999999999</v>
+        <v>42.959899999999998</v>
       </c>
       <c r="F6">
-        <v>31.696982999999999</v>
+        <v>31.943999999999999</v>
       </c>
       <c r="G6">
         <v>48.97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>400</v>
+      </c>
+      <c r="B2">
+        <v>395.94959999999998</v>
+      </c>
+      <c r="C2">
+        <v>167.7329</v>
+      </c>
+      <c r="D2">
+        <v>165.946</v>
+      </c>
+      <c r="E2">
+        <v>62.270699999999998</v>
+      </c>
+      <c r="F2">
+        <v>31.905000000000001</v>
+      </c>
+      <c r="G2">
+        <v>46.42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>375</v>
+      </c>
+      <c r="B3">
+        <v>371.80160000000001</v>
+      </c>
+      <c r="C3">
+        <v>160.328</v>
+      </c>
+      <c r="D3">
+        <v>150.84219999999999</v>
+      </c>
+      <c r="E3">
+        <v>60.631399999999999</v>
+      </c>
+      <c r="F3">
+        <v>31.606000000000002</v>
+      </c>
+      <c r="G3">
+        <v>46.89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>350</v>
+      </c>
+      <c r="B4">
+        <v>346.36559999999997</v>
+      </c>
+      <c r="C4">
+        <v>151.97880000000001</v>
+      </c>
+      <c r="D4">
+        <v>135.626</v>
+      </c>
+      <c r="E4">
+        <v>58.760799999999897</v>
+      </c>
+      <c r="F4">
+        <v>31.265999999999998</v>
+      </c>
+      <c r="G4">
+        <v>47.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>325</v>
+      </c>
+      <c r="B5">
+        <v>326.1336</v>
+      </c>
+      <c r="C5">
+        <v>146.1568</v>
+      </c>
+      <c r="D5">
+        <v>123.107</v>
+      </c>
+      <c r="E5">
+        <v>56.869799999999998</v>
+      </c>
+      <c r="F5">
+        <v>31.032</v>
+      </c>
+      <c r="G5">
+        <v>47.85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>300</v>
+      </c>
+      <c r="B6">
+        <v>310.63119999999998</v>
+      </c>
+      <c r="C6">
+        <v>140.22559999999999</v>
+      </c>
+      <c r="D6">
+        <v>116.687699999999</v>
+      </c>
+      <c r="E6">
+        <v>53.7179</v>
+      </c>
+      <c r="F6">
+        <v>30.742000000000001</v>
+      </c>
+      <c r="G6">
+        <v>48.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>